<commit_message>
Initial TTS and TTLE calibration
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7039CA60-D7B7-45DD-960C-8F19AB04F3D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="1785" windowWidth="28560" windowHeight="19110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24060" yWindow="1785" windowWidth="28560" windowHeight="19110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
     <sheet name="TTLE" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -97,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
@@ -806,39 +805,39 @@
     <cellStyle name="Accent5" xfId="48" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="52" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="21" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Body: normal cell" xfId="2" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Body: normal cell" xfId="2"/>
     <cellStyle name="Calculation" xfId="25" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Data" xfId="13" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Data no deci" xfId="59" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Data" xfId="13"/>
+    <cellStyle name="Data no deci" xfId="59"/>
     <cellStyle name="Explanatory Text" xfId="30" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="8" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Footnotes: all except top row" xfId="11" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="6" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="8"/>
+    <cellStyle name="Footnotes: all except top row" xfId="11"/>
+    <cellStyle name="Footnotes: top row" xfId="6"/>
     <cellStyle name="Good" xfId="20" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Header: bottom row" xfId="1" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Header: top rows" xfId="3" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Header: bottom row" xfId="1"/>
+    <cellStyle name="Header: top rows" xfId="3"/>
     <cellStyle name="Heading 1" xfId="16" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="17" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="18" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="19" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hed Side" xfId="14" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="58" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Hed Top" xfId="57" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Hyperlink 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Hed Side" xfId="14"/>
+    <cellStyle name="Hed Side Regular" xfId="58"/>
+    <cellStyle name="Hed Top" xfId="57"/>
+    <cellStyle name="Hyperlink 2" xfId="9"/>
     <cellStyle name="Input" xfId="23" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="26" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="22" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="29" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="24" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Section Break" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Section Break: parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Table title" xfId="12" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Parent row" xfId="5"/>
+    <cellStyle name="Section Break" xfId="7"/>
+    <cellStyle name="Section Break: parent row" xfId="4"/>
+    <cellStyle name="Table title" xfId="12"/>
     <cellStyle name="Title" xfId="15" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Title-2" xfId="56" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Title-2" xfId="56"/>
     <cellStyle name="Total" xfId="31" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="28" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -869,7 +868,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Table Style 1" pivot="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -961,23 +960,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1013,23 +995,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1205,22 +1170,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="45.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1228,194 +1193,194 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="27" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="1"/>
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B62" s="2"/>
     </row>
   </sheetData>
@@ -1425,22 +1390,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.59765625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -1451,70 +1418,70 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C2" s="4">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C3" s="4">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C4" s="4">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C5" s="4">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C6" s="4">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C7" s="4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3.4.3 --> 3.4.4 updating trans/TTLE (match GCAM values)
</commit_message>
<xml_diff>
--- a/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
+++ b/InputData/trans/TTLE/Transportation Technology Logit Exponents.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\trans\TTLE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\trans\TTLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368BEB8D-0281-414A-9219-6B1C7CD0D9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24060" yWindow="1785" windowWidth="28560" windowHeight="19110" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
-    <sheet name="TTLE" sheetId="10" r:id="rId2"/>
+    <sheet name="A54.tranSubsector_logit_revised" sheetId="11" r:id="rId2"/>
+    <sheet name="TTLE" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>ships</t>
   </si>
@@ -66,9 +68,6 @@
     <t>Logit exponent</t>
   </si>
   <si>
-    <t>None needed.  Handled through calibration.</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -91,12 +90,156 @@
   </si>
   <si>
     <t>https://jgcri.github.io/gcam-doc/choice.html</t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>We use the value from PNNL's GCAM model across vehicle technologies.</t>
+  </si>
+  <si>
+    <t># File: A54.tranSubsector_logit_revised.csv</t>
+  </si>
+  <si>
+    <t># Title: Transportation default subsector logit exponents</t>
+  </si>
+  <si>
+    <t># Source: Documented in JIRA issue https://jira.pnnl.gov/jira/browse/JGCRI-358?src=confmacro.</t>
+  </si>
+  <si>
+    <t># Units: Unitless</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Column types: ccicc </t>
+  </si>
+  <si>
+    <t># ----------</t>
+  </si>
+  <si>
+    <t>supplysector</t>
+  </si>
+  <si>
+    <t>tranSubsector</t>
+  </si>
+  <si>
+    <t>logit.exponent</t>
+  </si>
+  <si>
+    <t>logit.factor</t>
+  </si>
+  <si>
+    <t>logit.type</t>
+  </si>
+  <si>
+    <t>trn_aviation_intl</t>
+  </si>
+  <si>
+    <t>International Aviation</t>
+  </si>
+  <si>
+    <t>absolute-cost-logit</t>
+  </si>
+  <si>
+    <t>trn_freight</t>
+  </si>
+  <si>
+    <t>Domestic Ship</t>
+  </si>
+  <si>
+    <t>Freight Rail</t>
+  </si>
+  <si>
+    <t>Fuel types and efficiency levels</t>
+  </si>
+  <si>
+    <t>trn_freight_road</t>
+  </si>
+  <si>
+    <t>Light truck</t>
+  </si>
+  <si>
+    <t>Fuel types</t>
+  </si>
+  <si>
+    <t>Medium truck</t>
+  </si>
+  <si>
+    <t>Heavy truck</t>
+  </si>
+  <si>
+    <t>trn_pass</t>
+  </si>
+  <si>
+    <t>Cycle</t>
+  </si>
+  <si>
+    <t>Domestic Aviation</t>
+  </si>
+  <si>
+    <t>HSR</t>
+  </si>
+  <si>
+    <t>Passenger Rail</t>
+  </si>
+  <si>
+    <t>Walk</t>
+  </si>
+  <si>
+    <t>trn_pass_road</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>trn_pass_road_LDV</t>
+  </si>
+  <si>
+    <t>2W and 3W</t>
+  </si>
+  <si>
+    <t>trn_pass_road_LDV_4W</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Fuel types and ICE efficiency levels</t>
+  </si>
+  <si>
+    <t>Large Car and Truck</t>
+  </si>
+  <si>
+    <t>Mini Car</t>
+  </si>
+  <si>
+    <t>trn_shipping_intl</t>
+  </si>
+  <si>
+    <t>International Ship</t>
+  </si>
+  <si>
+    <t># Passthrough tranSubsectors are listed belowabsolute-cost-logit</t>
+  </si>
+  <si>
+    <t>road</t>
+  </si>
+  <si>
+    <t>LDV</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>4W</t>
+  </si>
+  <si>
+    <t>2W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="#,##0_)"/>
@@ -766,18 +909,15 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="60">
     <cellStyle name="20% - Accent1" xfId="33" builtinId="30" customBuiltin="1"/>
@@ -805,39 +945,39 @@
     <cellStyle name="Accent5" xfId="48" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="52" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="21" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Body: normal cell" xfId="2"/>
+    <cellStyle name="Body: normal cell" xfId="2" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
     <cellStyle name="Calculation" xfId="25" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Data" xfId="13"/>
-    <cellStyle name="Data no deci" xfId="59"/>
+    <cellStyle name="Data" xfId="13" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Data no deci" xfId="59" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="Explanatory Text" xfId="30" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="8"/>
-    <cellStyle name="Footnotes: all except top row" xfId="11"/>
-    <cellStyle name="Footnotes: top row" xfId="6"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="8" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="11" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="6" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
     <cellStyle name="Good" xfId="20" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Header: bottom row" xfId="1"/>
-    <cellStyle name="Header: top rows" xfId="3"/>
+    <cellStyle name="Header: bottom row" xfId="1" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Header: top rows" xfId="3" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Heading 1" xfId="16" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="17" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="18" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="19" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hed Side" xfId="14"/>
-    <cellStyle name="Hed Side Regular" xfId="58"/>
-    <cellStyle name="Hed Top" xfId="57"/>
-    <cellStyle name="Hyperlink 2" xfId="9"/>
+    <cellStyle name="Hed Side" xfId="14" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="58" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Hed Top" xfId="57" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="Input" xfId="23" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="26" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="22" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="29" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="24" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Parent row" xfId="5"/>
-    <cellStyle name="Section Break" xfId="7"/>
-    <cellStyle name="Section Break: parent row" xfId="4"/>
-    <cellStyle name="Table title" xfId="12"/>
+    <cellStyle name="Parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Section Break" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Section Break: parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Table title" xfId="12" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
     <cellStyle name="Title" xfId="15" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Title-2" xfId="56"/>
+    <cellStyle name="Title-2" xfId="56" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
     <cellStyle name="Total" xfId="31" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="28" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -868,7 +1008,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2">
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -960,6 +1100,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -995,6 +1152,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1170,218 +1344,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.3984375" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="27" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B62" s="2"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1390,98 +1424,534 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97FB3F6-A063-4685-A6D1-3D6F2007ED8F}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>-6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9">
+        <v>-6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>-8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12">
+        <v>-8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>-8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>-6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>-6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16">
+        <v>-6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17">
+        <v>-1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>-6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>-3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20">
+        <v>-8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21">
+        <v>-8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22">
+        <v>-8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23">
+        <v>-8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24">
+        <v>-6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>-6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27">
+        <v>-6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>-6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29">
+        <v>-6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30">
+        <v>-6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31">
+        <v>-6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4">
-        <v>-2</v>
-      </c>
-      <c r="C2" s="4">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B2">
+        <f>'A54.tranSubsector_logit_revised'!C21</f>
+        <v>-8</v>
+      </c>
+      <c r="C2">
+        <f>'A54.tranSubsector_logit_revised'!C11</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
-        <v>-2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <f>'A54.tranSubsector_logit_revised'!C19</f>
+        <v>-3</v>
+      </c>
+      <c r="C3">
+        <f>'A54.tranSubsector_logit_revised'!C13</f>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <v>-2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <f>'A54.tranSubsector_logit_revised'!C15</f>
+        <v>-6</v>
+      </c>
+      <c r="C4">
+        <f>'A54.tranSubsector_logit_revised'!C8</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
-        <v>-2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B5">
+        <f>'A54.tranSubsector_logit_revised'!C17</f>
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <f>'A54.tranSubsector_logit_revised'!C10</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4">
-        <v>-2</v>
-      </c>
-      <c r="C6" s="4">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B6">
+        <f>'A54.tranSubsector_logit_revised'!C24</f>
+        <v>-6</v>
+      </c>
+      <c r="C6">
+        <f>'A54.tranSubsector_logit_revised'!C9</f>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
-        <v>-2</v>
-      </c>
-      <c r="C7" s="4">
-        <v>-2</v>
+      <c r="B7">
+        <f>'A54.tranSubsector_logit_revised'!C20</f>
+        <v>-8</v>
+      </c>
+      <c r="C7">
+        <f>'A54.tranSubsector_logit_revised'!C20</f>
+        <v>-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>